<commit_message>
Commits to Jul 15 changes
</commit_message>
<xml_diff>
--- a/style_guide/acronyms_labels_notation.xlsx
+++ b/style_guide/acronyms_labels_notation.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie\Dropbox\1 Stat Project\teaching\open_intro\oi_biostat\style_guide\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26024"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19020" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="acronyms" sheetId="2" r:id="rId1"/>
     <sheet name="labels" sheetId="3" r:id="rId2"/>
     <sheet name="notation" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="83">
   <si>
     <t>acronym</t>
   </si>
@@ -224,6 +222,57 @@
   </si>
   <si>
     <t>exercise, identify target population</t>
+  </si>
+  <si>
+    <t>basicExampleOfPeanutAllergies</t>
+  </si>
+  <si>
+    <t>Case study from LEAP trial</t>
+  </si>
+  <si>
+    <t>peanutStudyResultsDF</t>
+  </si>
+  <si>
+    <t>results for 5 studies from LEAP</t>
+  </si>
+  <si>
+    <t>peanutStudyResults</t>
+  </si>
+  <si>
+    <t>summary of LEAP outcome</t>
+  </si>
+  <si>
+    <t>basicExampleOfFrogAltitude</t>
+  </si>
+  <si>
+    <t>Chen, et al paper on maternal investment</t>
+  </si>
+  <si>
+    <t>FrogAltitudeDF</t>
+  </si>
+  <si>
+    <t>sample data matrix for frog altitude data</t>
+  </si>
+  <si>
+    <t>famuss_height_weight</t>
+  </si>
+  <si>
+    <t>scatterplot of height vs weight</t>
+  </si>
+  <si>
+    <t>famuss_height_bmi</t>
+  </si>
+  <si>
+    <t>scatterplot of height vs bmi</t>
+  </si>
+  <si>
+    <t>table of 4 cases from famuss</t>
+  </si>
+  <si>
+    <t>FAMuSS_subset_Variables</t>
+  </si>
+  <si>
+    <t>definitions in famuss</t>
   </si>
 </sst>
 </file>
@@ -356,7 +405,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -391,7 +440,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -568,7 +617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -582,14 +631,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="26" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16" thickTop="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -605,7 +654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -613,7 +662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -621,7 +670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -629,7 +678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -637,7 +686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
@@ -645,7 +694,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -653,7 +702,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
@@ -663,26 +712,31 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="34.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="24" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -693,7 +747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" thickTop="1">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -704,7 +758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -715,7 +769,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -726,7 +780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -737,7 +791,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -748,7 +802,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -759,7 +813,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -770,7 +824,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -781,7 +835,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -792,7 +846,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
@@ -803,7 +857,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
@@ -814,7 +868,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
@@ -825,7 +879,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -836,7 +890,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
@@ -847,7 +901,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
@@ -858,7 +912,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
@@ -869,7 +923,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
         <v>58</v>
       </c>
@@ -880,7 +934,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
         <v>60</v>
       </c>
@@ -891,7 +945,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -902,7 +956,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>64</v>
       </c>
@@ -913,9 +967,113 @@
         <v>65</v>
       </c>
     </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -925,8 +1083,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
forgot to  update style guide
</commit_message>
<xml_diff>
--- a/style_guide/acronyms_labels_notation.xlsx
+++ b/style_guide/acronyms_labels_notation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19020" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25780" windowHeight="17820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="acronyms" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
   <si>
     <t>acronym</t>
   </si>
@@ -273,6 +273,18 @@
   </si>
   <si>
     <t>definitions in famuss</t>
+  </si>
+  <si>
+    <t>famussWeightDotPlotRobustEx</t>
+  </si>
+  <si>
+    <t>sdAsRuleForFrogAltitudeClutchVolume</t>
+  </si>
+  <si>
+    <t>dot plot of clutch.volume</t>
+  </si>
+  <si>
+    <t>dot plot of weights</t>
   </si>
 </sst>
 </file>
@@ -617,7 +629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -722,10 +734,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1064,6 +1076,28 @@
       </c>
       <c r="C30" s="2" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
frequent commits from Cambridge
</commit_message>
<xml_diff>
--- a/style_guide/acronyms_labels_notation.xlsx
+++ b/style_guide/acronyms_labels_notation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
   <si>
     <t>acronym</t>
   </si>
@@ -285,6 +285,18 @@
   </si>
   <si>
     <t>dot plot of weights</t>
+  </si>
+  <si>
+    <t>measuresOfCenter</t>
+  </si>
+  <si>
+    <t>Note change from OI, careful about future refs</t>
+  </si>
+  <si>
+    <t>measuresOfSpread</t>
+  </si>
+  <si>
+    <t>Note change from OI</t>
   </si>
 </sst>
 </file>
@@ -629,7 +641,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -734,10 +746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1098,6 +1110,28 @@
       </c>
       <c r="C32" s="2" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>